<commit_message>
download is in progress
</commit_message>
<xml_diff>
--- a/Api/uploads/users.xlsx
+++ b/Api/uploads/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Score</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t>Jithender</t>
   </si>
   <si>
@@ -46,9 +49,15 @@
     <t>jithender@yopmail.com</t>
   </si>
   <si>
+    <t>http://localhost:4200/results?id=6144200ecfd3d269458aa88c</t>
+  </si>
+  <si>
     <t>NA</t>
   </si>
   <si>
+    <t>http://localhost:4200/results?id=614428ab99333c7815ff3305</t>
+  </si>
+  <si>
     <t>Kapil</t>
   </si>
   <si>
@@ -61,10 +70,64 @@
     <t>kapil@ptg.com</t>
   </si>
   <si>
+    <t>http://localhost:4200/results?id=6144556972ca0e44448728d2</t>
+  </si>
+  <si>
     <t>Testin</t>
   </si>
   <si>
     <t>test.test@test.com</t>
+  </si>
+  <si>
+    <t>http://localhost:4200/results?id=614898fea455b3444460a516</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Smarketer</t>
+  </si>
+  <si>
+    <t>IT &amp; ITeS</t>
+  </si>
+  <si>
+    <t>test@Smarketer.com</t>
+  </si>
+  <si>
+    <t>http://localhost:4200/results?id=615d4cc96fe93130045395c3</t>
+  </si>
+  <si>
+    <t>Professional Services</t>
+  </si>
+  <si>
+    <t>http://localhost:4200/results?id=615d4d646fe93130045395d2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapil </t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>ED Cast</t>
+  </si>
+  <si>
+    <t>Kapil@edcast.com</t>
+  </si>
+  <si>
+    <t>http://localhost:4200/results?id=615d52796fe93130045395dc</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Conglomerate</t>
+  </si>
+  <si>
+    <t>kondurijithender@gmail.com</t>
+  </si>
+  <si>
+    <t>http://localhost:4200/results?id=616028fd8988fcc11153b3f7</t>
   </si>
 </sst>
 </file>
@@ -445,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
@@ -453,9 +516,10 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="204" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,85 +538,192 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
       <c r="F3">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>NaN</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>72</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>NaN</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>